<commit_message>
Changes for year 2018
</commit_message>
<xml_diff>
--- a/fi.semantum.strategia/database.xlsx
+++ b/fi.semantum.strategia/database.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18348" windowHeight="4416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Years</t>
   </si>
@@ -22,55 +23,7 @@
     <t>Monivalinta</t>
   </si>
   <si>
-    <t>Kyllä</t>
-  </si>
-  <si>
-    <t>Ei</t>
-  </si>
-  <si>
-    <t>Kyllä/Ei</t>
-  </si>
-  <si>
-    <t>Valtion tulostietojärjestelmä</t>
-  </si>
-  <si>
-    <t>Tavoite ylitetty</t>
-  </si>
-  <si>
-    <t>Tavoite saavutettu</t>
-  </si>
-  <si>
-    <t>Toteutui osittain</t>
-  </si>
-  <si>
     <t>Ei toteutunut</t>
-  </si>
-  <si>
-    <t>Ei aloitettu / tavoitteesta luovuttu</t>
-  </si>
-  <si>
-    <t>Hallituksen vuosikertomus</t>
-  </si>
-  <si>
-    <t>Erinomainen</t>
-  </si>
-  <si>
-    <t>Hyvä</t>
-  </si>
-  <si>
-    <t>Tyydyttävä</t>
-  </si>
-  <si>
-    <t>Välttävä</t>
-  </si>
-  <si>
-    <t>Aloittamatta/heikko</t>
-  </si>
-  <si>
-    <t>vp</t>
-  </si>
-  <si>
-    <t>vvkpp</t>
   </si>
   <si>
     <t>Toteuma</t>
@@ -88,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,6 +166,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,6 +218,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,21 +414,21 @@
   <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -458,95 +445,29 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>